<commit_message>
Aggiunto i Paesi Bassi
</commit_message>
<xml_diff>
--- a/legislature.xlsx
+++ b/legislature.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Documents\GitHub\legislature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F9ECCE-1D59-42A6-9145-A4BE78826C52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81A3F2E-8FF4-4E4B-B349-101C10B96698}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" xr2:uid="{0AA036FD-B706-457C-9E38-E1111F2A78BC}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="23040" windowHeight="12204" xr2:uid="{0AA036FD-B706-457C-9E38-E1111F2A78BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="85">
   <si>
     <t>paese</t>
   </si>
@@ -244,12 +244,60 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/October_1959_Icelandic_parliamentary_election</t>
+  </si>
+  <si>
+    <t>Paesi Bassi</t>
+  </si>
+  <si>
+    <t>Scioglimento anticipato per poter approvare riforma costituzionale postcoloniale</t>
+  </si>
+  <si>
+    <t>Caduta del governo Drees III</t>
+  </si>
+  <si>
+    <t>Caduta governo Cals</t>
+  </si>
+  <si>
+    <t>Prime elezioni senza voto obbligatorio</t>
+  </si>
+  <si>
+    <t>Caduta governo Biesheuvel I</t>
+  </si>
+  <si>
+    <t>Mandato prolungato per scioglimento anticipato</t>
+  </si>
+  <si>
+    <t>Caduta governo Van Agt II</t>
+  </si>
+  <si>
+    <t>Caduta governo per rapporto su Srebrenica ma a camere quasi sciolte</t>
+  </si>
+  <si>
+    <t>Caduta governo Balkenende I</t>
+  </si>
+  <si>
+    <t>Caduta governo Balkenende II, non si erano estesi il mandato a 5 anni</t>
+  </si>
+  <si>
+    <t>Caduta Balkenende IV, si erano estesi il mandato a 5</t>
+  </si>
+  <si>
+    <t>Caduta governo Rutte I, non si erano estesi il mandato</t>
+  </si>
+  <si>
+    <t>Mandato prolungato per scioglimento anticipato, Rutte II primo governo da Kok I a fare un interno mandato parlamentare</t>
+  </si>
+  <si>
+    <t>Caduta governo Rutte III, elezioni non anticipate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -285,20 +333,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="20" formatCode="dd\-mmm\-yy"/>
+      <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="20" formatCode="dd\-mmm\-yy"/>
+      <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -314,8 +363,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{714C403F-AF67-41FE-B455-D5B93BEA0AAB}" name="Tabella1" displayName="Tabella1" ref="A1:I181" totalsRowShown="0">
-  <autoFilter ref="A1:I181" xr:uid="{57565825-99DD-4E25-888D-A8B563A6201A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{714C403F-AF67-41FE-B455-D5B93BEA0AAB}" name="Tabella1" displayName="Tabella1" ref="A1:I204" totalsRowShown="0">
+  <autoFilter ref="A1:I204" xr:uid="{57565825-99DD-4E25-888D-A8B563A6201A}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{618F1481-1CB5-4F15-A26B-ADBF71E98623}" name="paese"/>
     <tableColumn id="6" xr3:uid="{1527285D-6DBC-449D-97C5-59B773E384CB}" name="assemblea"/>
@@ -332,7 +381,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -628,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB721021-4E39-4ED1-AF37-73AC7FFEE469}">
-  <dimension ref="A1:I181"/>
+  <dimension ref="A1:I204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="92" workbookViewId="0">
-      <selection activeCell="I172" sqref="I172"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4496,6 +4545,534 @@
         <v>68</v>
       </c>
     </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>70</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="D182" s="3">
+        <v>16939</v>
+      </c>
+      <c r="E182" s="3">
+        <v>17721</v>
+      </c>
+      <c r="F182">
+        <v>4</v>
+      </c>
+      <c r="G182" t="s">
+        <v>35</v>
+      </c>
+      <c r="H182" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>70</v>
+      </c>
+      <c r="C183">
+        <v>2</v>
+      </c>
+      <c r="D183" s="3">
+        <f>E182</f>
+        <v>17721</v>
+      </c>
+      <c r="E183" s="3">
+        <v>19170</v>
+      </c>
+      <c r="F183">
+        <v>4</v>
+      </c>
+      <c r="G183" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>70</v>
+      </c>
+      <c r="C184">
+        <v>3</v>
+      </c>
+      <c r="D184" s="3">
+        <f t="shared" ref="D184:D204" si="4">E183</f>
+        <v>19170</v>
+      </c>
+      <c r="E184" s="3">
+        <v>20619</v>
+      </c>
+      <c r="F184">
+        <v>4</v>
+      </c>
+      <c r="G184" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>70</v>
+      </c>
+      <c r="C185">
+        <v>4</v>
+      </c>
+      <c r="D185" s="3">
+        <f t="shared" si="4"/>
+        <v>20619</v>
+      </c>
+      <c r="E185" s="3">
+        <v>21621</v>
+      </c>
+      <c r="F185">
+        <v>4</v>
+      </c>
+      <c r="G185" t="s">
+        <v>35</v>
+      </c>
+      <c r="H185" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>70</v>
+      </c>
+      <c r="C186">
+        <f>C185+1</f>
+        <v>5</v>
+      </c>
+      <c r="D186" s="3">
+        <f t="shared" si="4"/>
+        <v>21621</v>
+      </c>
+      <c r="E186" s="3">
+        <v>23146</v>
+      </c>
+      <c r="F186">
+        <v>4</v>
+      </c>
+      <c r="G186" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>70</v>
+      </c>
+      <c r="C187">
+        <f t="shared" ref="C187:C203" si="5">C186+1</f>
+        <v>6</v>
+      </c>
+      <c r="D187" s="3">
+        <f t="shared" si="4"/>
+        <v>23146</v>
+      </c>
+      <c r="E187" s="3">
+        <v>24518</v>
+      </c>
+      <c r="F187">
+        <v>4</v>
+      </c>
+      <c r="G187" t="s">
+        <v>35</v>
+      </c>
+      <c r="H187" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>70</v>
+      </c>
+      <c r="C188">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="D188" s="3">
+        <f t="shared" si="4"/>
+        <v>24518</v>
+      </c>
+      <c r="E188" s="3">
+        <v>26051</v>
+      </c>
+      <c r="F188">
+        <v>4</v>
+      </c>
+      <c r="G188" t="s">
+        <v>35</v>
+      </c>
+      <c r="H188" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>70</v>
+      </c>
+      <c r="C189">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="D189" s="3">
+        <f t="shared" si="4"/>
+        <v>26051</v>
+      </c>
+      <c r="E189" s="3">
+        <v>26632</v>
+      </c>
+      <c r="F189">
+        <v>4</v>
+      </c>
+      <c r="G189" t="s">
+        <v>35</v>
+      </c>
+      <c r="H189" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>70</v>
+      </c>
+      <c r="C190">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="D190" s="3">
+        <f t="shared" si="4"/>
+        <v>26632</v>
+      </c>
+      <c r="E190" s="3">
+        <v>28270</v>
+      </c>
+      <c r="F190">
+        <v>5</v>
+      </c>
+      <c r="G190" t="s">
+        <v>35</v>
+      </c>
+      <c r="H190" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>70</v>
+      </c>
+      <c r="C191">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="D191" s="3">
+        <f t="shared" si="4"/>
+        <v>28270</v>
+      </c>
+      <c r="E191" s="3">
+        <v>29732</v>
+      </c>
+      <c r="F191">
+        <v>4</v>
+      </c>
+      <c r="G191" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>70</v>
+      </c>
+      <c r="C192">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="D192" s="3">
+        <f t="shared" si="4"/>
+        <v>29732</v>
+      </c>
+      <c r="E192" s="3">
+        <v>30202</v>
+      </c>
+      <c r="F192">
+        <v>4</v>
+      </c>
+      <c r="G192" t="s">
+        <v>35</v>
+      </c>
+      <c r="H192" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>70</v>
+      </c>
+      <c r="C193">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="D193" s="3">
+        <f t="shared" si="4"/>
+        <v>30202</v>
+      </c>
+      <c r="E193" s="3">
+        <v>31553</v>
+      </c>
+      <c r="F193">
+        <v>4</v>
+      </c>
+      <c r="G193" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>70</v>
+      </c>
+      <c r="C194">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="D194" s="3">
+        <f t="shared" si="4"/>
+        <v>31553</v>
+      </c>
+      <c r="E194" s="3">
+        <v>32757</v>
+      </c>
+      <c r="F194">
+        <v>4</v>
+      </c>
+      <c r="G194" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>70</v>
+      </c>
+      <c r="C195">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="D195" s="3">
+        <f t="shared" si="4"/>
+        <v>32757</v>
+      </c>
+      <c r="E195" s="3">
+        <v>34457</v>
+      </c>
+      <c r="F195">
+        <v>5</v>
+      </c>
+      <c r="G195" t="s">
+        <v>35</v>
+      </c>
+      <c r="H195" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>70</v>
+      </c>
+      <c r="C196">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="D196" s="3">
+        <f t="shared" si="4"/>
+        <v>34457</v>
+      </c>
+      <c r="E196" s="3">
+        <v>35921</v>
+      </c>
+      <c r="F196">
+        <v>4</v>
+      </c>
+      <c r="G196" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>70</v>
+      </c>
+      <c r="C197">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="D197" s="3">
+        <f t="shared" si="4"/>
+        <v>35921</v>
+      </c>
+      <c r="E197" s="3">
+        <v>37391</v>
+      </c>
+      <c r="F197">
+        <v>4</v>
+      </c>
+      <c r="G197" t="s">
+        <v>35</v>
+      </c>
+      <c r="H197" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>70</v>
+      </c>
+      <c r="C198">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="D198" s="3">
+        <f t="shared" si="4"/>
+        <v>37391</v>
+      </c>
+      <c r="E198" s="3">
+        <v>37643</v>
+      </c>
+      <c r="F198">
+        <v>4</v>
+      </c>
+      <c r="G198" t="s">
+        <v>35</v>
+      </c>
+      <c r="H198" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>70</v>
+      </c>
+      <c r="C199">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="D199" s="3">
+        <f t="shared" si="4"/>
+        <v>37643</v>
+      </c>
+      <c r="E199" s="3">
+        <v>39043</v>
+      </c>
+      <c r="F199">
+        <v>4</v>
+      </c>
+      <c r="G199" t="s">
+        <v>35</v>
+      </c>
+      <c r="H199" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>70</v>
+      </c>
+      <c r="C200">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="D200" s="3">
+        <f t="shared" si="4"/>
+        <v>39043</v>
+      </c>
+      <c r="E200" s="3">
+        <v>40338</v>
+      </c>
+      <c r="F200">
+        <v>5</v>
+      </c>
+      <c r="G200" t="s">
+        <v>35</v>
+      </c>
+      <c r="H200" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>70</v>
+      </c>
+      <c r="C201">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="D201" s="3">
+        <f t="shared" si="4"/>
+        <v>40338</v>
+      </c>
+      <c r="E201" s="3">
+        <v>41164</v>
+      </c>
+      <c r="F201">
+        <v>4</v>
+      </c>
+      <c r="G201" t="s">
+        <v>35</v>
+      </c>
+      <c r="H201" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>70</v>
+      </c>
+      <c r="C202">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="D202" s="3">
+        <f t="shared" si="4"/>
+        <v>41164</v>
+      </c>
+      <c r="E202" s="3">
+        <v>43034</v>
+      </c>
+      <c r="F202">
+        <v>5</v>
+      </c>
+      <c r="G202" t="s">
+        <v>35</v>
+      </c>
+      <c r="H202" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>70</v>
+      </c>
+      <c r="C203">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="D203" s="3">
+        <f t="shared" si="4"/>
+        <v>43034</v>
+      </c>
+      <c r="E203" s="3">
+        <v>44272</v>
+      </c>
+      <c r="F203">
+        <v>4</v>
+      </c>
+      <c r="G203" t="s">
+        <v>35</v>
+      </c>
+      <c r="H203" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D204" s="3"/>
+      <c r="E204" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>